<commit_message>
Put Johhny's code into MATLAB file
 plus other minor updates
</commit_message>
<xml_diff>
--- a/MATLAB/backscatterPlots.xlsx
+++ b/MATLAB/backscatterPlots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunet-my.sharepoint.com/personal/phbm_lunet_lboro_ac_uk/Documents/M_PHC902_GroupProject/MATLABCode/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunet-my.sharepoint.com/personal/phbm_lunet_lboro_ac_uk/Documents/M_PHC902_GroupProject/GitRepoSea/TeamSeaCode/MATLAB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_F25DC773A252ABDACC10489441DB63725BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8679DD45-FA4A-4314-8BBE-7C05EE0E7624}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="11_F25DC773A252ABDACC10489441DB63725BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79E32C3C-3FB0-4E10-B87B-16F9EEF8FFFE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="8565" yWindow="1425" windowWidth="11160" windowHeight="9015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -63,7 +63,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{5944DFD0-3F6B-42CD-8089-F20C76F57F1F}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -96,7 +98,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="4000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -109,14 +111,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB" sz="2400"/>
+              <a:rPr lang="en-GB" sz="4000" b="1"/>
               <a:t>Backscatter</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-GB" sz="2400" baseline="0"/>
+              <a:rPr lang="en-GB" sz="4000" b="1" baseline="0"/>
               <a:t> Data</a:t>
             </a:r>
-            <a:endParaRPr lang="en-GB" sz="2400"/>
+            <a:endParaRPr lang="en-GB" sz="4000" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -133,7 +135,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="4000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -151,7 +153,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11841841193207854"/>
+          <c:y val="8.9406166490031469E-2"/>
+          <c:w val="0.82848813747630756"/>
+          <c:h val="0.79930988312078188"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -159,7 +171,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -3222,6 +3234,7 @@
         <c:axId val="866332448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="500"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3239,6 +3252,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="2800"/>
+                  <a:t>Sample number (Simulation</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="2800" baseline="0"/>
+                  <a:t> step)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="2800"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3261,7 +3334,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3284,6 +3357,8 @@
         <c:axId val="866332776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2.5000000000000005E-3"/>
+          <c:min val="-1.4000000000000002E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3301,6 +3376,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="2800"/>
+                  <a:t>Pressure</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="2800" baseline="0"/>
+                  <a:t> Amplitude</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="2800"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3323,7 +3458,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3954,16 +4089,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>338139</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>23813</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4256,8 +4391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C502"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C502" sqref="B3:C502"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AK38" sqref="AK38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>